<commit_message>
Changes done in Every Execution Classes and Write Code for Pass n Fail
</commit_message>
<xml_diff>
--- a/BookStore/External Files/Book1.xlsx
+++ b/BookStore/External Files/Book1.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="21015" windowHeight="11250"/>
+    <workbookView activeTab="1" windowHeight="10275" windowWidth="11430" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet4" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:I32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>SI No</t>
   </si>
@@ -122,12 +123,16 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -180,25 +185,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -207,10 +212,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -366,7 +371,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -375,13 +380,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -391,7 +396,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -400,7 +405,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -409,7 +414,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -419,12 +424,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -455,7 +460,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -474,7 +479,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -487,19 +492,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -568,7 +573,7 @@
         <v>4575</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -591,34 +596,35 @@
         <v>54210</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="D3"/>
+    <hyperlink r:id="rId2" ref="D4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId3" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,8 +634,11 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -639,8 +648,11 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -650,31 +662,34 @@
       <c r="C3">
         <v>1234</v>
       </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -708,7 +723,9 @@
       <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
@@ -741,10 +758,13 @@
       <c r="J2" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -756,6 +776,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>